<commit_message>
test result document parser added
</commit_message>
<xml_diff>
--- a/public/sample_downloads/test_result_sample.xlsx
+++ b/public/sample_downloads/test_result_sample.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>class_room</t>
   </si>
   <si>
+    <t>section</t>
+  </si>
+  <si>
     <t>student_name</t>
   </si>
   <si>
@@ -41,13 +44,16 @@
     <t>roll_no</t>
   </si>
   <si>
+    <t>year</t>
+  </si>
+  <si>
     <t>remarks</t>
   </si>
   <si>
-    <t>1A</t>
-  </si>
-  <si>
-    <t>Jhon</t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Shivling</t>
   </si>
   <si>
     <t>Physics</t>
@@ -62,6 +68,9 @@
     <t>FA1</t>
   </si>
   <si>
+    <t>2012-2013</t>
+  </si>
+  <si>
     <t>Need improvement in core concepts</t>
   </si>
   <si>
@@ -71,22 +80,16 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>A</t>
+    <t>2011-2013</t>
   </si>
   <si>
     <t>Good, Kee it up.</t>
   </si>
   <si>
-    <t>1B</t>
-  </si>
-  <si>
     <t>Keyn</t>
   </si>
   <si>
     <t>A+</t>
-  </si>
-  <si>
-    <t>fail</t>
   </si>
   <si>
     <t>Very Good</t>
@@ -99,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -119,12 +122,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -169,17 +166,9 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -199,135 +188,166 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5867346938776"/>
-    <col collapsed="false" hidden="false" max="8" min="3" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.7857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.8826530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.40816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.76530612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.4591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.01020408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.51530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="6.8469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="30.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="C2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>56</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>83.5</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>83.5</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="n">
+      <c r="I3" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
+      <c r="J3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>88</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>88</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="2" t="n">
-        <v>13</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
+      <c r="K4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>